<commit_message>
update manual tcs and format it
</commit_message>
<xml_diff>
--- a/hoanghamobile/src/resources/Team_08_Manual_TCs.xlsx
+++ b/hoanghamobile/src/resources/Team_08_Manual_TCs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Home_Page" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="209">
   <si>
     <t>TCs</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>1.Chọn vào chức năng Tra cứu đơn hàng trên thanh Menu</t>
+  </si>
+  <si>
+    <t>4.Quay lại trang chủ</t>
+  </si>
+  <si>
+    <t>2.Quay lại trang chủ</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -786,99 +792,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -888,7 +801,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -901,7 +814,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -912,10 +825,40 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -923,18 +866,44 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -943,23 +912,47 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -972,8 +965,12 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -984,84 +981,13 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -1080,7 +1006,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1092,24 +1018,38 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1122,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1135,144 +1075,129 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1556,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1582,741 +1507,741 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="43" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="44" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="44" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="44" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="44" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="45" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="45" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="45" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="14" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="45" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="45" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="45" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="45" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="45" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="45" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="45" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="45" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="27"/>
+      <c r="D21" s="32"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="45" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="45" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="32"/>
     </row>
     <row r="24" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="45" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="45" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="32"/>
     </row>
     <row r="26" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="45" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="32"/>
     </row>
     <row r="28" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="45" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="45" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="32"/>
     </row>
     <row r="30" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="45" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="45" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="32"/>
     </row>
     <row r="32" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="45" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="45" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="27"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="45" t="s">
+      <c r="A34" s="38"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="45" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="27"/>
+      <c r="D35" s="32"/>
     </row>
     <row r="36" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="45" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="45" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="27"/>
+      <c r="D37" s="32"/>
     </row>
     <row r="38" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="45" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="45" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="45" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="45" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="27"/>
+      <c r="D42" s="32"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="48" t="s">
+      <c r="A43" s="40"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="31"/>
+      <c r="D43" s="47"/>
     </row>
     <row r="44" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="45" t="s">
+      <c r="A44" s="38"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="45" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="27"/>
+      <c r="D45" s="32"/>
     </row>
     <row r="46" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="45" t="s">
+      <c r="A46" s="38"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="45" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="45" t="s">
+      <c r="C47" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="45" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="45" t="s">
+      <c r="C48" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="45" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="45" t="s">
+      <c r="C49" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="45" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="45" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="45" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="45" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="45" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="45" t="s">
+      <c r="C54" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="45" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="30" t="s">
+      <c r="D55" s="45" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="45" t="s">
+      <c r="C56" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="45" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C57" s="45" t="s">
+      <c r="C57" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="45" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C58" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="45" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C59" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="45" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2328,7 +2253,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2353,100 +2278,100 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="47" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="34" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="47" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="45" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="34" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="32"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="47" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="47" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="45" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="36" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2565,10 +2490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2593,147 +2518,209 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="42" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="43" t="s">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B6" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C6" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B8" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C8" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="9" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B10" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C10" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="11" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B12" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C12" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+    <row r="13" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B14" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C14" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D14" s="22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="15" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B16" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C16" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D16" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+    <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
+  <mergeCells count="14">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>